<commit_message>
SWAP Nodes in Linkedlist
</commit_message>
<xml_diff>
--- a/SWEpreparation.xlsx
+++ b/SWEpreparation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programms\programming\Python\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1A3D4C-E242-46D9-A95A-9E7A0B3E4A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232EB1EA-3C74-4831-BBDA-E46D40D32E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="120">
   <si>
     <t>problem</t>
   </si>
@@ -1274,6 +1274,59 @@
       </rPr>
       <t> </t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>14.2 MB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF455A64"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>, less than </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF263238"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>76.64%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>32 ms</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF455A64"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>, faster than </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF263238"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>69.36%</t>
+    </r>
+  </si>
+  <si>
+    <t>25 Swap Nodes</t>
   </si>
 </sst>
 </file>
@@ -1624,7 +1677,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2335,8 +2388,34 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B26" s="3"/>
+    <row r="26" spans="1:9" ht="24" x14ac:dyDescent="0.45">
+      <c r="A26" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26" s="3">
+        <v>44467</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B27" s="3"/>

</xml_diff>

<commit_message>
Task 26 remove element
</commit_message>
<xml_diff>
--- a/SWEpreparation.xlsx
+++ b/SWEpreparation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programms\programming\Python\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0B7DBA-A595-462A-A95B-D21F1698221F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03243863-0272-4976-9D0A-7736758E7461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="130">
   <si>
     <t>problem</t>
   </si>
@@ -1452,6 +1452,72 @@
         <charset val="204"/>
       </rPr>
       <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>27 remove_Element</t>
+  </si>
+  <si>
+    <t>1ч 30 мин</t>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF263238"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>28 ms</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF455A64"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>, faster than </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF263238"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>93.96%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>14.2 MB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF455A64"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>, less than </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF263238"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>47.40%</t>
     </r>
   </si>
 </sst>
@@ -1802,8 +1868,8 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2391,7 +2457,7 @@
       <c r="G21" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="12" t="s">
         <v>99</v>
       </c>
       <c r="I21" s="16" t="s">
@@ -2420,7 +2486,7 @@
       <c r="G22" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H22" s="16" t="s">
+      <c r="H22" s="12" t="s">
         <v>103</v>
       </c>
       <c r="I22" s="16" t="s">
@@ -2478,7 +2544,7 @@
       <c r="G24" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="H24" s="12" t="s">
         <v>111</v>
       </c>
       <c r="I24" s="16" t="s">
@@ -2507,7 +2573,7 @@
       <c r="G25" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="H25" s="13" t="s">
         <v>114</v>
       </c>
       <c r="I25" s="16" t="s">
@@ -2536,7 +2602,7 @@
       <c r="G26" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H26" s="16" t="s">
+      <c r="H26" s="12" t="s">
         <v>117</v>
       </c>
       <c r="I26" s="16" t="s">
@@ -2601,8 +2667,34 @@
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B29" s="3"/>
+    <row r="29" spans="1:9" ht="24" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="3">
+        <v>44471</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B30" s="3"/>

</xml_diff>

<commit_message>
First and Last positions
</commit_message>
<xml_diff>
--- a/SWEpreparation.xlsx
+++ b/SWEpreparation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programms\programming\Python\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269CE554-965F-44EE-AE49-04656BAE5F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962730C2-0FDF-4A9C-A427-25F81FED9E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="158">
   <si>
     <t>problem</t>
   </si>
@@ -1868,6 +1868,59 @@
   </si>
   <si>
     <t>33 search-in-rotated-sorted-array</t>
+  </si>
+  <si>
+    <t>34_Find_First_and_Last_Position</t>
+  </si>
+  <si>
+    <r>
+      <t>15.2 MB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF455A64"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>, less than </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF263238"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>99.83%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>88 ms</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF455A64"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>, faster than </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF263238"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>55.33%</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2260,8 +2313,8 @@
   </sheetPr>
   <dimension ref="A1:J999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="B29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3359,8 +3412,37 @@
         <v>153</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B35" s="3"/>
+    <row r="35" spans="1:10" ht="24" x14ac:dyDescent="0.45">
+      <c r="A35" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="B35" s="3">
+        <v>44510</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I35" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="J35" s="14" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B36" s="3"/>

</xml_diff>

<commit_message>
35 search and insert position
</commit_message>
<xml_diff>
--- a/SWEpreparation.xlsx
+++ b/SWEpreparation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programms\programming\Python\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962730C2-0FDF-4A9C-A427-25F81FED9E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E403BBB-D6D1-46D5-AC51-589624A7F44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="162">
   <si>
     <t>problem</t>
   </si>
@@ -1921,6 +1921,69 @@
       </rPr>
       <t>55.33%</t>
     </r>
+  </si>
+  <si>
+    <t>35 Search_and_insert</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF263238"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>4.8 MB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF455A64"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>, less than </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF263238"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>94.77%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>52 ms</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF455A64"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>, faster than </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF263238"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>51.55%</t>
+    </r>
+  </si>
+  <si>
+    <t>bst, АиСД</t>
   </si>
 </sst>
 </file>
@@ -2313,8 +2376,8 @@
   </sheetPr>
   <dimension ref="A1:J999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3444,8 +3507,34 @@
         <v>156</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B36" s="3"/>
+    <row r="36" spans="1:10" ht="24" x14ac:dyDescent="0.45">
+      <c r="A36" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="B36" s="3">
+        <v>44527</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="J36" s="13" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B37" s="3"/>

</xml_diff>